<commit_message>
Documented code and printed output to Excel file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merna\Dropbox (SLG)\SunLight Energy Group Sales (shared)\Sunlight Energy Group - Merna shared\BGE Bill Extraction\BGE-Bill-Extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8028ADDB-4674-4035-9170-9E208477085E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B381ADF-3AF6-4EA1-97EF-199D6C6093D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,24 +450,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Deleted redundant cell definitions and added capability to save all data to same Excel file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,120 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merna\Dropbox (SLG)\SunLight Energy Group Sales (shared)\Sunlight Energy Group - Merna shared\BGE Bill Extraction\BGE-Bill-Extraction\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B381ADF-3AF6-4EA1-97EF-199D6C6093D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>utility</t>
-  </si>
-  <si>
-    <t>issued_date</t>
-  </si>
-  <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>street</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>zip_code</t>
-  </si>
-  <si>
-    <t>electric_choice_id</t>
-  </si>
-  <si>
-    <t>rate_code</t>
-  </si>
-  <si>
-    <t>electric_supplier</t>
-  </si>
-  <si>
-    <t>usage</t>
-  </si>
-  <si>
-    <t>BGE</t>
-  </si>
-  <si>
-    <t>November 23, 2020</t>
-  </si>
-  <si>
-    <t>Pharmaceutics International Inc</t>
-  </si>
-  <si>
-    <t>10947 Golden-West Dr *PS</t>
-  </si>
-  <si>
-    <t>Cockeysville</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>21030</t>
-  </si>
-  <si>
-    <t>5700075826</t>
-  </si>
-  <si>
-    <t>Schedule GL</t>
-  </si>
-  <si>
-    <t>Constellation New Energy, Inc</t>
-  </si>
-  <si>
-    <t>89744</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -122,44 +41,85 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -447,94 +407,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>BGE</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>September 18, 2020</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Pharmaceutics International Inc</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>10947 Golden-West Dr *PS</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Cockeysville</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MD</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>21030</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>5700075826</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Schedule GL</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Constellation New Energy, Inc</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>kWh</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>5700075825</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Schedule C</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>1075</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>